<commit_message>
Clean up xls file
</commit_message>
<xml_diff>
--- a/home/tests/import-export-data/assessment_empty_values.xlsx
+++ b/home/tests/import-export-data/assessment_empty_values.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="50">
   <si>
     <t xml:space="preserve">title</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t xml:space="preserve">dma_form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mnch_onboarding_dma_form</t>
   </si>
   <si>
     <t xml:space="preserve">English</t>
@@ -236,7 +239,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -279,13 +282,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Google Sans Mono"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -351,7 +347,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -392,32 +388,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -498,15 +470,15 @@
     <tabColor rgb="FFFF00FF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AH1000"/>
+  <dimension ref="A1:AM1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -598,476 +570,651 @@
       <c r="AH1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="10" t="str">
-        <f aca="false">LEFT(LOWER(CONCATENATE("mnch_onboarding_",A2)),LEN(LOWER(CONCATENATE("mnch_onboarding_",A2)))-3)</f>
-        <v>mnch_onboarding_dma_form</v>
+      <c r="C2" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="11" t="n">
+      <c r="X2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="11" t="n">
+      <c r="AB2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="1" t="s">
+      <c r="AD2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="E3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="K3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM3" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM4" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM5" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM6" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="13" t="s">
+      <c r="L7" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="N7" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="O7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3" t="s">
+      <c r="P7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="R7" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="9"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="S7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="U7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="V7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="10" t="str">
-        <f aca="false">LEFT(LOWER(CONCATENATE("mnch_onboarding_",A3)),LEN(LOWER(CONCATENATE("mnch_onboarding_",A3)))-3)</f>
-        <v>mnch_onboarding_dma_form</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="W7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="11" t="n">
+      <c r="X7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="11" t="n">
+      <c r="AB7" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="3" t="s">
+      <c r="AD7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="13" t="s">
+      <c r="AF7" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="AH7" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="AI7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="9"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="10" t="str">
-        <f aca="false">LEFT(LOWER(CONCATENATE("mnch_onboarding_",A4)),LEN(LOWER(CONCATENATE("mnch_onboarding_",A4)))-3)</f>
-        <v>mnch_onboarding_dma_form</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="15"/>
-      <c r="AG4" s="15"/>
-      <c r="AH4" s="9"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="10" t="str">
-        <f aca="false">LEFT(LOWER(CONCATENATE("mnch_onboarding_",A5)),LEN(LOWER(CONCATENATE("mnch_onboarding_",A5)))-3)</f>
-        <v>mnch_onboarding_dma_form</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="3"/>
-      <c r="N5" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="10"/>
-      <c r="AB5" s="10"/>
-      <c r="AC5" s="10"/>
-      <c r="AD5" s="10"/>
-      <c r="AE5" s="14"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
-      <c r="AH5" s="9"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="10" t="str">
-        <f aca="false">LEFT(LOWER(CONCATENATE("mnch_onboarding_",A6)),LEN(LOWER(CONCATENATE("mnch_onboarding_",A6)))-3)</f>
-        <v>mnch_onboarding_dma_form</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="10"/>
-      <c r="AB6" s="10"/>
-      <c r="AC6" s="10"/>
-      <c r="AD6" s="10"/>
-      <c r="AE6" s="14"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="10"/>
-      <c r="AA7" s="10"/>
-      <c r="AB7" s="10"/>
-      <c r="AC7" s="10"/>
-      <c r="AD7" s="10"/>
-      <c r="AE7" s="14"/>
+      <c r="AJ7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM7" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="A8" s="8"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10"/>
-      <c r="AA8" s="10"/>
-      <c r="AB8" s="10"/>
-      <c r="AC8" s="10"/>
-      <c r="AD8" s="10"/>
-      <c r="AE8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16"/>
+      <c r="A9" s="8"/>
       <c r="D9" s="3"/>
-      <c r="K9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16"/>
+      <c r="A10" s="8"/>
       <c r="D10" s="3"/>
-      <c r="K10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16"/>
+      <c r="A11" s="8"/>
       <c r="D11" s="3"/>
-      <c r="K11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16"/>
+      <c r="A12" s="8"/>
       <c r="D12" s="3"/>
-      <c r="K12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16"/>
+      <c r="A13" s="8"/>
       <c r="D13" s="3"/>
-      <c r="K13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16"/>
+      <c r="A14" s="8"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16"/>
+      <c r="A15" s="8"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16"/>
+      <c r="A16" s="8"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16"/>
+      <c r="A17" s="8"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16"/>
+      <c r="A18" s="8"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16"/>
+      <c r="A19" s="8"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16"/>
+      <c r="A20" s="8"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16"/>
+      <c r="A21" s="8"/>
       <c r="D21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16"/>
+      <c r="A22" s="8"/>
       <c r="D22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1754,114 +1901,33 @@
       <c r="A193" s="8"/>
       <c r="D193" s="3"/>
     </row>
-    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A194" s="8"/>
-      <c r="D194" s="3"/>
-    </row>
-    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A195" s="8"/>
-      <c r="D195" s="3"/>
-    </row>
-    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A196" s="8"/>
-      <c r="D196" s="3"/>
-    </row>
-    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A197" s="8"/>
-      <c r="D197" s="3"/>
-    </row>
-    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A198" s="8"/>
-      <c r="D198" s="3"/>
-    </row>
-    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A199" s="8"/>
-      <c r="D199" s="3"/>
-    </row>
-    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A200" s="8"/>
-      <c r="D200" s="3"/>
-    </row>
-    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A201" s="8"/>
-      <c r="D201" s="3"/>
-    </row>
-    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A202" s="8"/>
-      <c r="D202" s="3"/>
-    </row>
-    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A203" s="8"/>
-      <c r="D203" s="3"/>
-    </row>
-    <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A204" s="8"/>
-      <c r="D204" s="3"/>
-    </row>
-    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A205" s="8"/>
-      <c r="D205" s="3"/>
-    </row>
-    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A206" s="8"/>
-      <c r="D206" s="3"/>
-    </row>
-    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A207" s="8"/>
-      <c r="D207" s="3"/>
-    </row>
-    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A208" s="8"/>
-      <c r="D208" s="3"/>
-    </row>
-    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A209" s="8"/>
-      <c r="D209" s="3"/>
-    </row>
-    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A210" s="8"/>
-      <c r="D210" s="3"/>
-    </row>
-    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A211" s="8"/>
-      <c r="D211" s="3"/>
-    </row>
-    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A212" s="8"/>
-      <c r="D212" s="3"/>
-    </row>
-    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A213" s="8"/>
-      <c r="D213" s="3"/>
-    </row>
-    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A214" s="8"/>
-      <c r="D214" s="3"/>
-    </row>
-    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A215" s="8"/>
-      <c r="D215" s="3"/>
-    </row>
-    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A216" s="8"/>
-      <c r="D216" s="3"/>
-    </row>
-    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A217" s="8"/>
-      <c r="D217" s="3"/>
-    </row>
-    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A218" s="8"/>
-      <c r="D218" s="3"/>
-    </row>
-    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A219" s="8"/>
-      <c r="D219" s="3"/>
-    </row>
-    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A220" s="8"/>
-      <c r="D220" s="3"/>
-    </row>
+    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2615,33 +2681,33 @@
     <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Move xls fix into global xlsx reader so other importers can use it
</commit_message>
<xml_diff>
--- a/home/tests/import-export-data/assessment_empty_values.xlsx
+++ b/home/tests/import-export-data/assessment_empty_values.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="50">
   <si>
     <t xml:space="preserve">title</t>
   </si>
@@ -239,7 +239,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -277,16 +277,8 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,13 +288,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFF3F3F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3F3F3"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -347,7 +333,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -372,20 +358,8 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -401,66 +375,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFF3F3F3"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -470,15 +384,15 @@
     <tabColor rgb="FFFF00FF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM1048576"/>
+  <dimension ref="A1:T973"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -493,6 +407,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="41.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="24.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1004" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -554,23 +469,9 @@
         <v>18</v>
       </c>
       <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -591,7 +492,7 @@
       <c r="J2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="L2" s="0" t="s">
@@ -612,51 +513,9 @@
       <c r="S2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="W2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z2" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL2" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM2" s="0" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -686,7 +545,7 @@
       <c r="J3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="7" t="s">
         <v>35</v>
       </c>
       <c r="L3" s="0" t="s">
@@ -707,60 +566,9 @@
       <c r="S3" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="W3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z3" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AA3" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC3" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE3" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL3" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM3" s="0" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -790,7 +598,7 @@
       <c r="J4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="7" t="s">
         <v>39</v>
       </c>
       <c r="L4" s="0" t="s">
@@ -811,60 +619,9 @@
       <c r="S4" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="V4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="W4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AA4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE4" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL4" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM4" s="0" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -894,7 +651,7 @@
       <c r="J5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="7" t="s">
         <v>43</v>
       </c>
       <c r="L5" s="0" t="s">
@@ -915,60 +672,9 @@
       <c r="S5" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="U5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="V5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="W5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AA5" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC5" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL5" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM5" s="0" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -998,7 +704,7 @@
       <c r="J6" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="7" t="s">
         <v>47</v>
       </c>
       <c r="L6" s="0" t="s">
@@ -1019,60 +725,9 @@
       <c r="S6" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="U6" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="V6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="W6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AA6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB6" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD6" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE6" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ6" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM6" s="0" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -1093,7 +748,7 @@
       <c r="J7" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="7" t="s">
         <v>24</v>
       </c>
       <c r="L7" s="0" t="s">
@@ -1114,791 +769,749 @@
       <c r="S7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="U7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="V7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="W7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z7" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH7" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI7" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM7" s="0" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8"/>
+      <c r="A8" s="6"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8"/>
+      <c r="A9" s="6"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
+      <c r="A10" s="6"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8"/>
+      <c r="A11" s="6"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8"/>
+      <c r="A12" s="6"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8"/>
+      <c r="A13" s="6"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
+      <c r="A14" s="6"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8"/>
+      <c r="A15" s="6"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
+      <c r="A16" s="6"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
+      <c r="A17" s="6"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8"/>
+      <c r="A18" s="6"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8"/>
+      <c r="A19" s="6"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8"/>
+      <c r="A20" s="6"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8"/>
+      <c r="A21" s="6"/>
       <c r="D21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8"/>
+      <c r="A22" s="6"/>
       <c r="D22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8"/>
+      <c r="A23" s="6"/>
       <c r="D23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8"/>
+      <c r="A24" s="6"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8"/>
+      <c r="A25" s="6"/>
       <c r="D25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8"/>
+      <c r="A26" s="6"/>
       <c r="D26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8"/>
+      <c r="A27" s="6"/>
       <c r="D27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8"/>
+      <c r="A28" s="6"/>
       <c r="D28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8"/>
+      <c r="A29" s="6"/>
       <c r="D29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8"/>
+      <c r="A30" s="6"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8"/>
+      <c r="A31" s="6"/>
       <c r="D31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8"/>
+      <c r="A32" s="6"/>
       <c r="D32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8"/>
+      <c r="A33" s="6"/>
       <c r="D33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8"/>
+      <c r="A34" s="6"/>
       <c r="D34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8"/>
+      <c r="A35" s="6"/>
       <c r="D35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8"/>
+      <c r="A36" s="6"/>
       <c r="D36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8"/>
+      <c r="A37" s="6"/>
       <c r="D37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8"/>
+      <c r="A38" s="6"/>
       <c r="D38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8"/>
+      <c r="A39" s="6"/>
       <c r="D39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8"/>
+      <c r="A40" s="6"/>
       <c r="D40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8"/>
+      <c r="A41" s="6"/>
       <c r="D41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8"/>
+      <c r="A42" s="6"/>
       <c r="D42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8"/>
+      <c r="A43" s="6"/>
       <c r="D43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8"/>
+      <c r="A44" s="6"/>
       <c r="D44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="8"/>
+      <c r="A45" s="6"/>
       <c r="D45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8"/>
+      <c r="A46" s="6"/>
       <c r="D46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8"/>
+      <c r="A47" s="6"/>
       <c r="D47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8"/>
+      <c r="A48" s="6"/>
       <c r="D48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8"/>
+      <c r="A49" s="6"/>
       <c r="D49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="8"/>
+      <c r="A50" s="6"/>
       <c r="D50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8"/>
+      <c r="A51" s="6"/>
       <c r="D51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8"/>
+      <c r="A52" s="6"/>
       <c r="D52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8"/>
+      <c r="A53" s="6"/>
       <c r="D53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8"/>
+      <c r="A54" s="6"/>
       <c r="D54" s="3"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="8"/>
+      <c r="A55" s="6"/>
       <c r="D55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8"/>
+      <c r="A56" s="6"/>
       <c r="D56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="8"/>
+      <c r="A57" s="6"/>
       <c r="D57" s="3"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="8"/>
+      <c r="A58" s="6"/>
       <c r="D58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="8"/>
+      <c r="A59" s="6"/>
       <c r="D59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="8"/>
+      <c r="A60" s="6"/>
       <c r="D60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="8"/>
+      <c r="A61" s="6"/>
       <c r="D61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8"/>
+      <c r="A62" s="6"/>
       <c r="D62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="8"/>
+      <c r="A63" s="6"/>
       <c r="D63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="8"/>
+      <c r="A64" s="6"/>
       <c r="D64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="8"/>
+      <c r="A65" s="6"/>
       <c r="D65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="8"/>
+      <c r="A66" s="6"/>
       <c r="D66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="8"/>
+      <c r="A67" s="6"/>
       <c r="D67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="8"/>
+      <c r="A68" s="6"/>
       <c r="D68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="8"/>
+      <c r="A69" s="6"/>
       <c r="D69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="8"/>
+      <c r="A70" s="6"/>
       <c r="D70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="8"/>
+      <c r="A71" s="6"/>
       <c r="D71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="8"/>
+      <c r="A72" s="6"/>
       <c r="D72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="8"/>
+      <c r="A73" s="6"/>
       <c r="D73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="8"/>
+      <c r="A74" s="6"/>
       <c r="D74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="8"/>
+      <c r="A75" s="6"/>
       <c r="D75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="8"/>
+      <c r="A76" s="6"/>
       <c r="D76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="8"/>
+      <c r="A77" s="6"/>
       <c r="D77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="8"/>
+      <c r="A78" s="6"/>
       <c r="D78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="8"/>
+      <c r="A79" s="6"/>
       <c r="D79" s="3"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="8"/>
+      <c r="A80" s="6"/>
       <c r="D80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="8"/>
+      <c r="A81" s="6"/>
       <c r="D81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="8"/>
+      <c r="A82" s="6"/>
       <c r="D82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="8"/>
+      <c r="A83" s="6"/>
       <c r="D83" s="3"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="8"/>
+      <c r="A84" s="6"/>
       <c r="D84" s="3"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="8"/>
+      <c r="A85" s="6"/>
       <c r="D85" s="3"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="8"/>
+      <c r="A86" s="6"/>
       <c r="D86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="8"/>
+      <c r="A87" s="6"/>
       <c r="D87" s="3"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="8"/>
+      <c r="A88" s="6"/>
       <c r="D88" s="3"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="8"/>
+      <c r="A89" s="6"/>
       <c r="D89" s="3"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="8"/>
+      <c r="A90" s="6"/>
       <c r="D90" s="3"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="8"/>
+      <c r="A91" s="6"/>
       <c r="D91" s="3"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="8"/>
+      <c r="A92" s="6"/>
       <c r="D92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="8"/>
+      <c r="A93" s="6"/>
       <c r="D93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="8"/>
+      <c r="A94" s="6"/>
       <c r="D94" s="3"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="8"/>
+      <c r="A95" s="6"/>
       <c r="D95" s="3"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="8"/>
+      <c r="A96" s="6"/>
       <c r="D96" s="3"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="8"/>
+      <c r="A97" s="6"/>
       <c r="D97" s="3"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="8"/>
+      <c r="A98" s="6"/>
       <c r="D98" s="3"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="8"/>
+      <c r="A99" s="6"/>
       <c r="D99" s="3"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="8"/>
+      <c r="A100" s="6"/>
       <c r="D100" s="3"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="8"/>
+      <c r="A101" s="6"/>
       <c r="D101" s="3"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="8"/>
+      <c r="A102" s="6"/>
       <c r="D102" s="3"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="8"/>
+      <c r="A103" s="6"/>
       <c r="D103" s="3"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="8"/>
+      <c r="A104" s="6"/>
       <c r="D104" s="3"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="8"/>
+      <c r="A105" s="6"/>
       <c r="D105" s="3"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="8"/>
+      <c r="A106" s="6"/>
       <c r="D106" s="3"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="8"/>
+      <c r="A107" s="6"/>
       <c r="D107" s="3"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="8"/>
+      <c r="A108" s="6"/>
       <c r="D108" s="3"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="8"/>
+      <c r="A109" s="6"/>
       <c r="D109" s="3"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="8"/>
+      <c r="A110" s="6"/>
       <c r="D110" s="3"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="8"/>
+      <c r="A111" s="6"/>
       <c r="D111" s="3"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="8"/>
+      <c r="A112" s="6"/>
       <c r="D112" s="3"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="8"/>
+      <c r="A113" s="6"/>
       <c r="D113" s="3"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="8"/>
+      <c r="A114" s="6"/>
       <c r="D114" s="3"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="8"/>
+      <c r="A115" s="6"/>
       <c r="D115" s="3"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="8"/>
+      <c r="A116" s="6"/>
       <c r="D116" s="3"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="8"/>
+      <c r="A117" s="6"/>
       <c r="D117" s="3"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="8"/>
+      <c r="A118" s="6"/>
       <c r="D118" s="3"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="8"/>
+      <c r="A119" s="6"/>
       <c r="D119" s="3"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="8"/>
+      <c r="A120" s="6"/>
       <c r="D120" s="3"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="8"/>
+      <c r="A121" s="6"/>
       <c r="D121" s="3"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="8"/>
+      <c r="A122" s="6"/>
       <c r="D122" s="3"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="8"/>
+      <c r="A123" s="6"/>
       <c r="D123" s="3"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="8"/>
+      <c r="A124" s="6"/>
       <c r="D124" s="3"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="8"/>
+      <c r="A125" s="6"/>
       <c r="D125" s="3"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="8"/>
+      <c r="A126" s="6"/>
       <c r="D126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="8"/>
+      <c r="A127" s="6"/>
       <c r="D127" s="3"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="8"/>
+      <c r="A128" s="6"/>
       <c r="D128" s="3"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="8"/>
+      <c r="A129" s="6"/>
       <c r="D129" s="3"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="8"/>
+      <c r="A130" s="6"/>
       <c r="D130" s="3"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="8"/>
+      <c r="A131" s="6"/>
       <c r="D131" s="3"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="8"/>
+      <c r="A132" s="6"/>
       <c r="D132" s="3"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="8"/>
+      <c r="A133" s="6"/>
       <c r="D133" s="3"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="8"/>
+      <c r="A134" s="6"/>
       <c r="D134" s="3"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="8"/>
+      <c r="A135" s="6"/>
       <c r="D135" s="3"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A136" s="8"/>
+      <c r="A136" s="6"/>
       <c r="D136" s="3"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="8"/>
+      <c r="A137" s="6"/>
       <c r="D137" s="3"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="8"/>
+      <c r="A138" s="6"/>
       <c r="D138" s="3"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="8"/>
+      <c r="A139" s="6"/>
       <c r="D139" s="3"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A140" s="8"/>
+      <c r="A140" s="6"/>
       <c r="D140" s="3"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="8"/>
+      <c r="A141" s="6"/>
       <c r="D141" s="3"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="8"/>
+      <c r="A142" s="6"/>
       <c r="D142" s="3"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="8"/>
+      <c r="A143" s="6"/>
       <c r="D143" s="3"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A144" s="8"/>
+      <c r="A144" s="6"/>
       <c r="D144" s="3"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="8"/>
+      <c r="A145" s="6"/>
       <c r="D145" s="3"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="8"/>
+      <c r="A146" s="6"/>
       <c r="D146" s="3"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="8"/>
+      <c r="A147" s="6"/>
       <c r="D147" s="3"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A148" s="8"/>
+      <c r="A148" s="6"/>
       <c r="D148" s="3"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A149" s="8"/>
+      <c r="A149" s="6"/>
       <c r="D149" s="3"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A150" s="8"/>
+      <c r="A150" s="6"/>
       <c r="D150" s="3"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A151" s="8"/>
+      <c r="A151" s="6"/>
       <c r="D151" s="3"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A152" s="8"/>
+      <c r="A152" s="6"/>
       <c r="D152" s="3"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A153" s="8"/>
+      <c r="A153" s="6"/>
       <c r="D153" s="3"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A154" s="8"/>
+      <c r="A154" s="6"/>
       <c r="D154" s="3"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A155" s="8"/>
+      <c r="A155" s="6"/>
       <c r="D155" s="3"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A156" s="8"/>
+      <c r="A156" s="6"/>
       <c r="D156" s="3"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A157" s="8"/>
+      <c r="A157" s="6"/>
       <c r="D157" s="3"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A158" s="8"/>
+      <c r="A158" s="6"/>
       <c r="D158" s="3"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A159" s="8"/>
+      <c r="A159" s="6"/>
       <c r="D159" s="3"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A160" s="8"/>
+      <c r="A160" s="6"/>
       <c r="D160" s="3"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A161" s="8"/>
+      <c r="A161" s="6"/>
       <c r="D161" s="3"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A162" s="8"/>
+      <c r="A162" s="6"/>
       <c r="D162" s="3"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A163" s="8"/>
+      <c r="A163" s="6"/>
       <c r="D163" s="3"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A164" s="8"/>
+      <c r="A164" s="6"/>
       <c r="D164" s="3"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A165" s="8"/>
+      <c r="A165" s="6"/>
       <c r="D165" s="3"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A166" s="8"/>
+      <c r="A166" s="6"/>
       <c r="D166" s="3"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A167" s="8"/>
+      <c r="A167" s="6"/>
       <c r="D167" s="3"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A168" s="8"/>
+      <c r="A168" s="6"/>
       <c r="D168" s="3"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A169" s="8"/>
+      <c r="A169" s="6"/>
       <c r="D169" s="3"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A170" s="8"/>
+      <c r="A170" s="6"/>
       <c r="D170" s="3"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A171" s="8"/>
+      <c r="A171" s="6"/>
       <c r="D171" s="3"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A172" s="8"/>
+      <c r="A172" s="6"/>
       <c r="D172" s="3"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A173" s="8"/>
+      <c r="A173" s="6"/>
       <c r="D173" s="3"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A174" s="8"/>
+      <c r="A174" s="6"/>
       <c r="D174" s="3"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A175" s="8"/>
+      <c r="A175" s="6"/>
       <c r="D175" s="3"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A176" s="8"/>
+      <c r="A176" s="6"/>
       <c r="D176" s="3"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A177" s="8"/>
+      <c r="A177" s="6"/>
       <c r="D177" s="3"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A178" s="8"/>
+      <c r="A178" s="6"/>
       <c r="D178" s="3"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A179" s="8"/>
+      <c r="A179" s="6"/>
       <c r="D179" s="3"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A180" s="8"/>
+      <c r="A180" s="6"/>
       <c r="D180" s="3"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A181" s="8"/>
+      <c r="A181" s="6"/>
       <c r="D181" s="3"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A182" s="8"/>
+      <c r="A182" s="6"/>
       <c r="D182" s="3"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A183" s="8"/>
+      <c r="A183" s="6"/>
       <c r="D183" s="3"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A184" s="8"/>
+      <c r="A184" s="6"/>
       <c r="D184" s="3"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A185" s="8"/>
+      <c r="A185" s="6"/>
       <c r="D185" s="3"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A186" s="8"/>
+      <c r="A186" s="6"/>
       <c r="D186" s="3"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A187" s="8"/>
+      <c r="A187" s="6"/>
       <c r="D187" s="3"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A188" s="8"/>
+      <c r="A188" s="6"/>
       <c r="D188" s="3"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A189" s="8"/>
+      <c r="A189" s="6"/>
       <c r="D189" s="3"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A190" s="8"/>
+      <c r="A190" s="6"/>
       <c r="D190" s="3"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A191" s="8"/>
+      <c r="A191" s="6"/>
       <c r="D191" s="3"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A192" s="8"/>
+      <c r="A192" s="6"/>
       <c r="D192" s="3"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A193" s="8"/>
+      <c r="A193" s="6"/>
       <c r="D193" s="3"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2681,33 +2294,6 @@
     <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>